<commit_message>
support multiple sheets now
</commit_message>
<xml_diff>
--- a/treasure.xlsx
+++ b/treasure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code2\treasure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3766FE0F-5A56-4A3E-9D57-C2E11171724D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0C5A30-7D67-46F9-8CCB-2E8111D4E637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23415" windowHeight="15480" activeTab="1" xr2:uid="{49891337-194D-405F-863C-A201D62D5504}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12375" windowHeight="15480" activeTab="1" xr2:uid="{49891337-194D-405F-863C-A201D62D5504}"/>
   </bookViews>
   <sheets>
     <sheet name="Wales" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
   <si>
     <t>Location</t>
   </si>
@@ -134,15 +134,6 @@
   </si>
   <si>
     <t>Silver annular brooch with niello decoration discovered February 2021</t>
-  </si>
-  <si>
-    <t>Location Coordinates</t>
-  </si>
-  <si>
-    <t>Likelihood %</t>
-  </si>
-  <si>
-    <t>Recommend Reason</t>
   </si>
   <si>
     <t>Very High</t>
@@ -255,7 +246,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,12 +273,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9.6"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9.6"/>
@@ -326,7 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -345,9 +330,6 @@
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -679,7 +661,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,150 +827,150 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD2E2C8D-CA85-4D68-8E37-EE11CCB1A06B}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" ht="57" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="200.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="D2" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="200.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+    </row>
+    <row r="3" spans="1:6" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.65</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="142.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="129" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="9">
-        <v>0.8</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="D5" s="8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="157.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="9">
-        <v>0.65</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="142.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="8" t="s">
+      <c r="C6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="156.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="9">
+      <c r="C7" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="10">
         <v>0.6</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="129" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="157.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="9">
-        <v>0.7</v>
-      </c>
-      <c r="E6" s="8" t="s">
+      <c r="E7" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F7" s="9" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="156.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="11">
-        <v>0.6</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add more treasures locations
</commit_message>
<xml_diff>
--- a/treasure.xlsx
+++ b/treasure.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code2\treasure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0C5A30-7D67-46F9-8CCB-2E8111D4E637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D0AB35-0B6B-47C6-81F7-C4D1DAB52C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12375" windowHeight="15480" activeTab="1" xr2:uid="{49891337-194D-405F-863C-A201D62D5504}"/>
   </bookViews>
   <sheets>
     <sheet name="Wales" sheetId="1" r:id="rId1"/>
-    <sheet name="North Ireland" sheetId="2" r:id="rId2"/>
+    <sheet name="Scotland" sheetId="4" r:id="rId2"/>
+    <sheet name="North Ireland" sheetId="2" r:id="rId3"/>
+    <sheet name="England" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="136">
   <si>
     <t>Location</t>
   </si>
@@ -240,6 +242,222 @@
   </si>
   <si>
     <t>Carrowdressex, Co. Down</t>
+  </si>
+  <si>
+    <t>Norfolk (Norwich area)</t>
+  </si>
+  <si>
+    <t>52°37'51"N, 1°17'50"E</t>
+  </si>
+  <si>
+    <t>Highest concentration of treasure finds in England; rich historical habitation</t>
+  </si>
+  <si>
+    <t>116 treasure finds annually; extensive agricultural land turning up artifacts regularly</t>
+  </si>
+  <si>
+    <t>Suffolk (Hoxne area)</t>
+  </si>
+  <si>
+    <t>52°20'33"N, 1°11'15"E</t>
+  </si>
+  <si>
+    <t>Site of largest Roman hoard in Britain; established pattern of significant finds</t>
+  </si>
+  <si>
+    <t>Hoxne Hoard valued at £4.5 million (2023 value); 65 treasure finds annually9</t>
+  </si>
+  <si>
+    <t>Essex (Chelmsford area)</t>
+  </si>
+  <si>
+    <t>51°44'10"N, 0°28'47"E</t>
+  </si>
+  <si>
+    <t>Second-highest concentration of treasure finds; rich Roman and medieval history</t>
+  </si>
+  <si>
+    <t>71 treasure finds annually; proximity to Roman settlements</t>
+  </si>
+  <si>
+    <t>Lincolnshire</t>
+  </si>
+  <si>
+    <t>53°12'00"N, 0°36'00"W</t>
+  </si>
+  <si>
+    <t>Moderate-High</t>
+  </si>
+  <si>
+    <t>Consistent pattern of significant finds; historical settlement area</t>
+  </si>
+  <si>
+    <t>59 treasure finds annually; agricultural landscape exposing artifacts</t>
+  </si>
+  <si>
+    <t>North Yorkshire</t>
+  </si>
+  <si>
+    <t>54°00'00"N, 1°30'00"W</t>
+  </si>
+  <si>
+    <t>Viking settlement area; previous discovery of Viking jewelry</t>
+  </si>
+  <si>
+    <t>Documented Viking jewelry finds; historical records of settlement patterns</t>
+  </si>
+  <si>
+    <t>Herefordshire</t>
+  </si>
+  <si>
+    <t>52°06'00"N, 2°42'00"W</t>
+  </si>
+  <si>
+    <t>Moderate</t>
+  </si>
+  <si>
+    <t>Roman settlement area; previous coin hoard discoveries</t>
+  </si>
+  <si>
+    <t>Recent discovery of Roman coin hoard; archaeological evidence of Roman occupation</t>
+  </si>
+  <si>
+    <t>Buckinghamshire</t>
+  </si>
+  <si>
+    <t>51°48'00"N, 0°48'00"W</t>
+  </si>
+  <si>
+    <t>Norman and Anglo-Saxon settlement area; previous coin finds</t>
+  </si>
+  <si>
+    <t>Documented discovery of Norman and Anglo-Saxon coins</t>
+  </si>
+  <si>
+    <t>Greenwich Park, London</t>
+  </si>
+  <si>
+    <t>51°28'48"N, 0°00'00"E</t>
+  </si>
+  <si>
+    <t>Anglo-Saxon burial site with documented finds; scheduled monument status</t>
+  </si>
+  <si>
+    <t>Archaeological excavations revealing Anglo-Saxon artifacts including glass beads, shields, and swords</t>
+  </si>
+  <si>
+    <t>Traprain Law, East Lothian</t>
+  </si>
+  <si>
+    <t>55°58'N, 2°41'W</t>
+  </si>
+  <si>
+    <t>Very High (53+ lb of Roman silver)</t>
+  </si>
+  <si>
+    <t>Proven site of significant Roman silver hoard</t>
+  </si>
+  <si>
+    <t>1919 discovery of a major Roman silver hoard, over 150 objects, 4th century AD</t>
+  </si>
+  <si>
+    <t>Carpow, River Tay-Earn</t>
+  </si>
+  <si>
+    <t>56°23'N, 3°17'W</t>
+  </si>
+  <si>
+    <t>Roman military fort, potential for further finds</t>
+  </si>
+  <si>
+    <t>Early 3rd-century Roman fort, previous finds include armor and amphorae</t>
+  </si>
+  <si>
+    <t>Moray Coast (Pictish Fort)</t>
+  </si>
+  <si>
+    <t>57°41'N, 3°18'W</t>
+  </si>
+  <si>
+    <t>Exceptional preservation from 10th-century fire</t>
+  </si>
+  <si>
+    <t>Recent excavations revealed a “treasure trove” of Pictish artifacts, jewelry, preserved wood</t>
+  </si>
+  <si>
+    <t>Balmaghie, Kirkcudbrightshire</t>
+  </si>
+  <si>
+    <t>54°56'N, 4°06'W</t>
+  </si>
+  <si>
+    <t>Very High (5+ kg silver/gold)</t>
+  </si>
+  <si>
+    <t>Cultural crossroads of Viking kingdoms</t>
+  </si>
+  <si>
+    <t>Galloway Hoard: 100+ objects of gold, silver, glass, crystal, stone, and clay from the Viking Age</t>
+  </si>
+  <si>
+    <t>Aberdeenshire (Hacksilver)</t>
+  </si>
+  <si>
+    <t>57°16'N, 2°22'W</t>
+  </si>
+  <si>
+    <t>High (100+ silver objects)</t>
+  </si>
+  <si>
+    <t>Part of a pattern of hacksilver hoard deposits</t>
+  </si>
+  <si>
+    <t>Late Roman hacksilver hoard with Roman and Pictish items, 4th–6th century CE</t>
+  </si>
+  <si>
+    <t>Peebles area</t>
+  </si>
+  <si>
+    <t>55°39'N, 3°11'W</t>
+  </si>
+  <si>
+    <t>£80,000 (officially valued)</t>
+  </si>
+  <si>
+    <t>Evidence of Bronze Age international connections</t>
+  </si>
+  <si>
+    <t>Bronze Age hoard of 500+ bronze/organic pieces, 1000–800 BCE, including rare rattle pendants</t>
+  </si>
+  <si>
+    <t>Trimontium, near Melrose</t>
+  </si>
+  <si>
+    <t>55°36'N, 2°43'W</t>
+  </si>
+  <si>
+    <t>Moderate to High</t>
+  </si>
+  <si>
+    <t>Major Roman settlement and industrial complex</t>
+  </si>
+  <si>
+    <t>Early 20th-century excavations found a wide range of well-preserved artifacts from waterlogged pits</t>
+  </si>
+  <si>
+    <t>Rosslyn Chapel, near Edinburgh</t>
+  </si>
+  <si>
+    <t>55°51'N, 3°09'W</t>
+  </si>
+  <si>
+    <t>Potentially Priceless (speculative)</t>
+  </si>
+  <si>
+    <t>Theoretical Holy Grail/Templar connection</t>
+  </si>
+  <si>
+    <t>Theories based on 15th-century scrolls and Templar legends, no confirmed discoveries</t>
   </si>
 </sst>
 </file>
@@ -694,7 +912,7 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -824,8 +1042,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD2E2C8D-CA85-4D68-8E37-EE11CCB1A06B}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5453FB5A-F1DA-4479-9535-F825EB0C404F}">
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:F1"/>
@@ -853,6 +1071,201 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0.65</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="157.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="186" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="186" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.35</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="186" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="185.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD2E2C8D-CA85-4D68-8E37-EE11CCB1A06B}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="57" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="2" spans="1:6" ht="200.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>53</v>
@@ -982,4 +1395,203 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7BC7723-9723-4CFD-B483-0D4E4F1763BA}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="57" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="157.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.85</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="143.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="143.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="143.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.65</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="157.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="129" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="199.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" display="https://en.wikipedia.org/wiki/Hoxne_Hoard" xr:uid="{68F717ED-C0B4-44F8-98D0-043591C9EF68}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>